<commit_message>
Added new functional PI requirements
</commit_message>
<xml_diff>
--- a/docs/Project Goals - Preliminary.xlsx
+++ b/docs/Project Goals - Preliminary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dio_g\Documents\Makerspace\Access Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dio_g\Source\Repos\GJMsAC\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{65AED346-F44C-4EF4-A1F8-F310CB3859DF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{4F8C2DD2-4E9D-4D60-83E4-59F6C8218ACE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16423" windowHeight="6574" xr2:uid="{6684E988-E0D3-4646-969A-A270BA9F5F0C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21446" windowHeight="11931" activeTab="1" xr2:uid="{6684E988-E0D3-4646-969A-A270BA9F5F0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Management" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="117">
   <si>
     <t>Description</t>
   </si>
@@ -357,6 +357,27 @@
   </si>
   <si>
     <t>Phone will support provider model for membership access</t>
+  </si>
+  <si>
+    <t>PI will be able to load configuration from SD card</t>
+  </si>
+  <si>
+    <t>PI will be able to load initial membership data from SD card</t>
+  </si>
+  <si>
+    <t>PI will be able to overwrite membership data on SD card with data from phone</t>
+  </si>
+  <si>
+    <t>PI will be able to overwrite membership data on SD card with data from network</t>
+  </si>
+  <si>
+    <t>PI will not allow access to SD card without special tools</t>
+  </si>
+  <si>
+    <t>PI will not allow access to SD card from locked side (that is side with RFID scanner)</t>
+  </si>
+  <si>
+    <t>PI will be able to overwrite membership data on SD card with data from membership provider</t>
   </si>
 </sst>
 </file>
@@ -470,14 +491,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -995,7 +1016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED93D6F-40CB-451F-9327-5222D0F4CAAD}">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1155,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FDF43C-CDBD-4719-BA1B-BAB812F38300}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1170,18 +1191,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45.45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
@@ -1667,6 +1688,62 @@
       </c>
       <c r="B67" s="3" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A68" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A69" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A70" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A71" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A72" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A73" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A74" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1697,18 +1774,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="29.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="20"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="20"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="20"/>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">

</xml_diff>